<commit_message>
Agregado del análisis de rendimiento y readme
</commit_message>
<xml_diff>
--- a/Proyecto02_v2/MundoParalelo/design/Análisis de speedup y eficiencia.xlsx
+++ b/Proyecto02_v2/MundoParalelo/design/Análisis de speedup y eficiencia.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24312"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C396DAC7-A6E8-48EB-913F-021F98359CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{45634273-BD55-4B9E-93D2-284E5FDE967A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2A31D13B-DD25-48E3-8AC4-EDCA9163F9F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -26,12 +34,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t>Mapeo</t>
+    <t>BOSQUE ENCANTADO (PARALELIZADO CON OMP Y DISTRIBUIDO CON MPI)</t>
   </si>
   <si>
-    <t>Tiempo</t>
+    <t>Versión</t>
+  </si>
+  <si>
+    <t>Cantidad de hilos</t>
+  </si>
+  <si>
+    <t>Cantidad de procesos</t>
+  </si>
+  <si>
+    <t>Duración (min)</t>
   </si>
   <si>
     <t>Speedup</t>
@@ -40,22 +57,16 @@
     <t>Eficiencia</t>
   </si>
   <si>
-    <t>Los cálculos de speedup y eficiencia fueron realizados en symbolab</t>
-  </si>
-  <si>
-    <t>Bloque</t>
-  </si>
-  <si>
-    <t>Guiado</t>
-  </si>
-  <si>
-    <t>Dinámico</t>
-  </si>
-  <si>
     <t>Serial</t>
   </si>
   <si>
-    <t>Job002</t>
+    <t>Distribuido MPI</t>
+  </si>
+  <si>
+    <t>Concurrente OMP</t>
+  </si>
+  <si>
+    <t>Híbrido OMP y MPI</t>
   </si>
 </sst>
 </file>
@@ -63,9 +74,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0.00000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,26 +85,55 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -103,158 +143,151 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FF002060"/>
       </left>
       <right style="thin">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FF002060"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FF002060"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FF002060"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF002060"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF002060"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF002060"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF002060"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FF002060"/>
       </left>
       <right style="thin">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FF002060"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
+      <top style="medium">
+        <color rgb="FF002060"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FF002060"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FF002060"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF002060"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF002060"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF002060"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF002060"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF002060"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF002060"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF002060"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF002060"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF002060"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF002060"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF002060"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF002060"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF002060"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF002060"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF002060"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF002060"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF002060"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF002060"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF002060"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF002060"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF002060"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF002060"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF002060"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF002060"/>
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FF002060"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FF002060"/>
       </bottom>
       <diagonal/>
     </border>
@@ -262,56 +295,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -357,8 +379,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Tiempos de duración por mapeo</a:t>
+              <a:rPr lang="es-CR"/>
+              <a:t>Eficiencia</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -395,23 +417,24 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="AEAAAA"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -442,6 +465,7 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="t"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -471,52 +495,42 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$B$8:$E$8</c:f>
+              <c:f>Hoja1!$B$6:$B$7</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Bloque</c:v>
+                  <c:v>Concurrente OMP</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Guiado</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Dinámico</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Serial</c:v>
+                  <c:v>Híbrido OMP y MPI</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$B$9:$E$9</c:f>
+              <c:f>Hoja1!$G$6:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>61.25</c:v>
+                  <c:v>0.23565</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>65.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>66.22</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>111.7</c:v>
+                  <c:v>0.29407</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-CB5F-45CF-82AD-4FF3DC13EEF7}"/>
+              <c16:uniqueId val="{00000000-08EF-4987-BEE3-3C2B781D1274}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
@@ -524,72 +538,17 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:axId val="1818723032"/>
-        <c:axId val="1450866440"/>
-      </c:barChart>
+        <c:smooth val="0"/>
+        <c:axId val="2132740399"/>
+        <c:axId val="2126971311"/>
+      </c:lineChart>
       <c:catAx>
-        <c:axId val="1818723032"/>
+        <c:axId val="2132740399"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Tipo de Mapeo</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -627,7 +586,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1450866440"/>
+        <c:crossAx val="2126971311"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -635,7 +594,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1450866440"/>
+        <c:axId val="2126971311"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -655,61 +614,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Tiempos de duración</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -741,7 +645,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1818723032"/>
+        <c:crossAx val="2132740399"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -755,6 +659,13 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -825,7 +736,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Incremento de velocidad por mapeo</a:t>
+              <a:t>Speedup</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -862,23 +773,24 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="AEAAAA"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -909,7 +821,7 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="outEnd"/>
+            <c:dLblPos val="t"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -939,47 +851,48 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$A$2:$A$4</c:f>
+              <c:f>Hoja1!$B$5:$B$7</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Bloque</c:v>
+                  <c:v>Distribuido MPI</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Guiado</c:v>
+                  <c:v>Concurrente OMP</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Dinámico</c:v>
+                  <c:v>Híbrido OMP y MPI</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$C$2:$C$4</c:f>
+              <c:f>Hoja1!$F$5:$F$7</c:f>
               <c:numCache>
-                <c:formatCode>#,##0.00000</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.8236699999999999</c:v>
+                  <c:v>1.35538</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.7053400000000001</c:v>
+                  <c:v>1.8852</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6868000000000001</c:v>
+                  <c:v>2.3526099999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E72F-4430-AB8C-02C24C45FFD4}"/>
+              <c16:uniqueId val="{00000001-86BC-4F22-B874-1108F728B5E4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
+          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
@@ -987,73 +900,17 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="425764504"/>
-        <c:axId val="777975176"/>
-      </c:barChart>
+        <c:smooth val="0"/>
+        <c:axId val="513249143"/>
+        <c:axId val="692177847"/>
+      </c:lineChart>
       <c:catAx>
-        <c:axId val="425764504"/>
+        <c:axId val="513249143"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Tipo de Mapeo</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1091,7 +948,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="777975176"/>
+        <c:crossAx val="692177847"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1099,7 +956,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="777975176"/>
+        <c:axId val="692177847"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1119,62 +976,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Speedup</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="#,##0.00000" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1205,7 +1007,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="425764504"/>
+        <c:crossAx val="513249143"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1289,7 +1091,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Eficiencia por mapeo</a:t>
+              <a:t>Tiempos de duración por versión</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1335,7 +1137,7 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="AEAAAA"/>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1403,42 +1205,42 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$A$2:$A$4</c:f>
+              <c:f>Hoja1!$B$5:$B$7</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Bloque</c:v>
+                  <c:v>Distribuido MPI</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Guiado</c:v>
+                  <c:v>Concurrente OMP</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Dinámico</c:v>
+                  <c:v>Híbrido OMP y MPI</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$D$2:$D$4</c:f>
+              <c:f>Hoja1!$E$5:$E$7</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.22795000000000001</c:v>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>82.412000000000006</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.21315999999999999</c:v>
+                  <c:v>59.251280000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.21085000000000001</c:v>
+                  <c:v>47.478679999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0287-42C0-9E8F-67D839795EBE}"/>
+              <c16:uniqueId val="{00000001-C57C-4806-AF68-908697986295}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1453,71 +1255,16 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="771308968"/>
-        <c:axId val="1995214504"/>
+        <c:axId val="201230984"/>
+        <c:axId val="1176854664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="771308968"/>
+        <c:axId val="201230984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Tipo de Mapeo</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1555,7 +1302,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1995214504"/>
+        <c:crossAx val="1176854664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1563,7 +1310,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1995214504"/>
+        <c:axId val="1176854664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1604,7 +1351,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Eficiencia</a:t>
+                  <a:t>Tiempo (min)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1669,7 +1416,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="771308968"/>
+        <c:crossAx val="201230984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1839,7 +1586,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1947,6 +1694,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -1957,6 +1709,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -1988,6 +1745,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2342,7 +2102,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2450,6 +2210,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -2460,6 +2225,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -2491,6 +2261,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3351,23 +3124,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>928687</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>747712</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="18" name="Gráfico 17">
+        <xdr:cNvPr id="8" name="Gráfico 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24E3A6B7-E97D-4A20-9D76-9136952FEC5E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD991A69-95A0-46A7-93B9-ECE3D47A3803}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{8B13E83F-9D5C-4FAC-932A-38AC083799FA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3385,28 +3161,122 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{485D27EE-DAC1-444F-B26D-70C6274335AA}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{FD991A69-95A0-46A7-93B9-ECE3D47A3803}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7477125" y="123825"/>
+          <a:ext cx="2676525" cy="752475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{273BBDB1-1C02-4F3F-9F72-AA13E128087F}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{485D27EE-DAC1-444F-B26D-70C6274335AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10106025" y="85725"/>
+          <a:ext cx="3181350" cy="752475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>771525</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="20" name="Gráfico 19">
+        <xdr:cNvPr id="4" name="Gráfico 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4F77334-DFE7-4239-ADB8-16F80C6B43FE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0C32E3B-9F7F-4D09-BF88-C1D06F152061}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{24E3A6B7-E97D-4A20-9D76-9136952FEC5E}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{273BBDB1-1C02-4F3F-9F72-AA13E128087F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3418,7 +3288,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3426,26 +3296,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="21" name="Gráfico 20">
+        <xdr:cNvPr id="5" name="Gráfico 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E89536E5-032A-41BC-A84D-DD9882C0C417}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E8BA336-C0BE-48DE-B279-044FD8C99B78}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{F4F77334-DFE7-4239-ADB8-16F80C6B43FE}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{F0C32E3B-9F7F-4D09-BF88-C1D06F152061}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3457,104 +3327,10 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7606927E-80BF-453A-8FCA-351BAD7BE519}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{E89536E5-032A-41BC-A84D-DD9882C0C417}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3162300" y="457200"/>
-          <a:ext cx="2038350" cy="571500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Imagen 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{799AFCE6-8AFB-4399-97F5-F907B75F432F}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{7606927E-80BF-453A-8FCA-351BAD7BE519}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5257800" y="476250"/>
-          <a:ext cx="2390775" cy="571500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3856,122 +3632,142 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF94E89A-68AF-4F95-9C1A-7B6E1A40795B}">
+  <dimension ref="B1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="2:7">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="11"/>
+    </row>
+    <row r="2" spans="2:7">
+      <c r="B2" s="12"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="14"/>
+    </row>
+    <row r="3" spans="2:7">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="4" t="s">
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="9">
-        <v>61.25</v>
-      </c>
-      <c r="C2" s="8">
-        <v>1.8236699999999999</v>
-      </c>
-      <c r="D2" s="10">
-        <v>0.22795000000000001</v>
+      <c r="G3" s="7" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="4" t="s">
-        <v>6</v>
+    <row r="4" spans="2:7">
+      <c r="B4" s="3" t="s">
+        <v>7</v>
       </c>
-      <c r="B3" s="9">
-        <v>65.5</v>
+      <c r="C4" s="15">
+        <v>1</v>
       </c>
-      <c r="C3" s="8">
-        <v>1.7053400000000001</v>
+      <c r="D4" s="15">
+        <v>1</v>
       </c>
-      <c r="D3" s="10">
-        <v>0.21315999999999999</v>
+      <c r="E4" s="15">
+        <v>111.7</v>
+      </c>
+      <c r="F4" s="15"/>
+      <c r="G4" s="16"/>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2">
+        <v>82.412000000000006</v>
+      </c>
+      <c r="F5" s="15">
+        <v>1.35538</v>
+      </c>
+      <c r="G5" s="19"/>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="17">
+        <v>59.251280000000001</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1.8852</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.23565</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="4" t="s">
-        <v>7</v>
+    <row r="7" spans="2:7" ht="15.75" thickBot="1">
+      <c r="B7" s="4" t="s">
+        <v>10</v>
       </c>
-      <c r="B4" s="9">
-        <v>66.22</v>
+      <c r="C7" s="5">
+        <v>8</v>
       </c>
-      <c r="C4" s="8">
-        <v>1.6868000000000001</v>
+      <c r="D7" s="5">
+        <v>3</v>
       </c>
-      <c r="D4" s="10">
-        <v>0.21085000000000001</v>
+      <c r="E7" s="18">
+        <v>47.478679999999997</v>
+      </c>
+      <c r="F7" s="5">
+        <v>2.3526099999999999</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0.29407</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="6">
-        <v>111.7</v>
-      </c>
-      <c r="C5" s="12">
-        <v>0</v>
-      </c>
-      <c r="D5" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="14.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14">
-        <v>61.25</v>
-      </c>
-      <c r="C9" s="14">
-        <v>65.5</v>
-      </c>
-      <c r="D9" s="14">
-        <v>66.22</v>
-      </c>
-      <c r="E9" s="14">
-        <v>111.7</v>
-      </c>
+    <row r="36" spans="7:7">
+      <c r="G36" s="8"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:G2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>